<commit_message>
results with precision values
</commit_message>
<xml_diff>
--- a/tarraxo/resultados.xlsx
+++ b/tarraxo/resultados.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CF78F15-B04F-4668-85B5-253059664732}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C7EDE2B-474E-4A8A-800E-0A199A4F15C9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="146">
   <si>
     <t>modelo</t>
   </si>
@@ -278,9 +278,6 @@
     <t>12.50%</t>
   </si>
   <si>
-    <t>86.22%</t>
-  </si>
-  <si>
     <t>80.15%</t>
   </si>
   <si>
@@ -297,13 +294,191 @@
   </si>
   <si>
     <t>41.67%</t>
+  </si>
+  <si>
+    <t>precision 0</t>
+  </si>
+  <si>
+    <t>precision 1</t>
+  </si>
+  <si>
+    <t>2.82%</t>
+  </si>
+  <si>
+    <t>87.34%</t>
+  </si>
+  <si>
+    <t>91.84%</t>
+  </si>
+  <si>
+    <t>92.41%</t>
+  </si>
+  <si>
+    <t>20.00%</t>
+  </si>
+  <si>
+    <t>91.95%</t>
+  </si>
+  <si>
+    <t>91.61%</t>
+  </si>
+  <si>
+    <t>90.62%</t>
+  </si>
+  <si>
+    <t>5.56%</t>
+  </si>
+  <si>
+    <t>89.58%</t>
+  </si>
+  <si>
+    <t>21.21%</t>
+  </si>
+  <si>
+    <t>98.44%</t>
+  </si>
+  <si>
+    <t>64.71%</t>
+  </si>
+  <si>
+    <t>88.51%</t>
+  </si>
+  <si>
+    <t>86.81%</t>
+  </si>
+  <si>
+    <t>27.78%</t>
+  </si>
+  <si>
+    <t>96.25%</t>
+  </si>
+  <si>
+    <t>25.61%</t>
+  </si>
+  <si>
+    <t>91.78%</t>
+  </si>
+  <si>
+    <t>75.00%</t>
+  </si>
+  <si>
+    <t>86.16%</t>
+  </si>
+  <si>
+    <t>86.25%</t>
+  </si>
+  <si>
+    <t>82.76%</t>
+  </si>
+  <si>
+    <t>95.05%</t>
+  </si>
+  <si>
+    <t>31.15%</t>
+  </si>
+  <si>
+    <t>85.81%</t>
+  </si>
+  <si>
+    <t>28.57%</t>
+  </si>
+  <si>
+    <t>84.62%</t>
+  </si>
+  <si>
+    <t>5.41%</t>
+  </si>
+  <si>
+    <t>90.24%</t>
+  </si>
+  <si>
+    <t>91.89%</t>
+  </si>
+  <si>
+    <t>91.49%</t>
+  </si>
+  <si>
+    <t>91.37%</t>
+  </si>
+  <si>
+    <t>80.56%</t>
+  </si>
+  <si>
+    <t>13.49%</t>
+  </si>
+  <si>
+    <t>92.98%</t>
+  </si>
+  <si>
+    <t>33.33%</t>
+  </si>
+  <si>
+    <t>85.44%</t>
+  </si>
+  <si>
+    <t>86.21%</t>
+  </si>
+  <si>
+    <t>23.53%</t>
+  </si>
+  <si>
+    <t>95.89%</t>
+  </si>
+  <si>
+    <t>23.60%</t>
+  </si>
+  <si>
+    <t>86.45%</t>
+  </si>
+  <si>
+    <t>42.86%</t>
+  </si>
+  <si>
+    <t>85.09%</t>
+  </si>
+  <si>
+    <t>85.22%</t>
+  </si>
+  <si>
+    <t>85.19%</t>
+  </si>
+  <si>
+    <t>90.15%</t>
+  </si>
+  <si>
+    <t>36.67%</t>
+  </si>
+  <si>
+    <t>89.71%</t>
+  </si>
+  <si>
+    <t>38.46%</t>
+  </si>
+  <si>
+    <t>85.00%</t>
+  </si>
+  <si>
+    <r>
+      <t>0.00</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>%</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -326,8 +501,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <strike/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -337,6 +520,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -470,23 +659,42 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="0" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="0" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="10" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="0" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="0" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -772,31 +980,33 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F43"/>
   <sheetViews>
-    <sheetView topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I40" sqref="I40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
     <col min="2" max="4" width="15.7265625" customWidth="1"/>
+    <col min="5" max="5" width="12.7265625" customWidth="1"/>
+    <col min="6" max="6" width="13.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A1" s="16" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1" s="35" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A2" s="16"/>
-      <c r="B2" s="16"/>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" s="35"/>
+      <c r="B2" s="35"/>
+      <c r="C2" s="35"/>
+      <c r="D2" s="35"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -809,23 +1019,35 @@
       <c r="D4" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A6" s="8" t="s">
+      <c r="E4" t="s">
+        <v>91</v>
+      </c>
+      <c r="F4" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A6" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="C6" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="D6" s="10" t="s">
+      <c r="D6" s="11" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E6" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="F6" s="12" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7" s="2" t="s">
         <v>11</v>
       </c>
@@ -835,45 +1057,63 @@
       <c r="C7" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="D7" s="4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="11"/>
-      <c r="B8" s="12"/>
-      <c r="C8" s="12"/>
-      <c r="D8" s="12"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A9" s="8" t="s">
+      <c r="D7" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E7" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="F7" s="19" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A8" s="8"/>
+      <c r="B8" s="9"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A9" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="9" t="s">
+      <c r="B9" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="C9" s="9" t="s">
+      <c r="C9" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="D9" s="10" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A10" s="5" t="s">
+      <c r="D9" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E9" s="21" t="s">
+        <v>95</v>
+      </c>
+      <c r="F9" s="22" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A10" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C10" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="D10" s="7" t="s">
+      <c r="D10" s="14" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E10" s="24" t="s">
+        <v>96</v>
+      </c>
+      <c r="F10" s="25" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="2" t="s">
         <v>14</v>
       </c>
@@ -883,141 +1123,189 @@
       <c r="C11" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="D11" s="3" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A12" s="11"/>
-      <c r="B12" s="11"/>
-      <c r="C12" s="11"/>
-      <c r="D12" s="11"/>
-    </row>
-    <row r="13" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="13" t="s">
+      <c r="E11" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="F11" s="19" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A12" s="8"/>
+      <c r="B12" s="8"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+    </row>
+    <row r="13" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A13" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="B13" s="14" t="s">
+      <c r="B13" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="C13" s="14" t="s">
+      <c r="C13" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="D13" s="15" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A14" s="11"/>
-      <c r="B14" s="11"/>
-      <c r="C14" s="11"/>
-      <c r="D14" s="11"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A15" s="8" t="s">
+      <c r="D13" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="E13" s="26" t="s">
+        <v>98</v>
+      </c>
+      <c r="F13" s="27" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A14" s="8"/>
+      <c r="B14" s="8"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A15" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B15" s="9" t="s">
+      <c r="B15" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="C15" s="9" t="s">
+      <c r="C15" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="D15" s="10" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A16" s="5" t="s">
+      <c r="D15" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E15" s="21" t="s">
+        <v>98</v>
+      </c>
+      <c r="F15" s="22" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A16" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B16" s="6" t="s">
+      <c r="B16" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C16" s="6" t="s">
+      <c r="C16" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D16" s="7" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A17" s="5" t="s">
+      <c r="D16" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="F16" s="23" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A17" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B17" s="6" t="s">
+      <c r="B17" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C17" s="6" t="s">
+      <c r="C17" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="D17" s="7" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A18" s="5" t="s">
+      <c r="D17" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="F17" s="23" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A18" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B18" s="6" t="s">
+      <c r="B18" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="C18" s="6" t="s">
+      <c r="C18" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="D18" s="7" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="2" t="s">
+      <c r="D18" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="F18" s="23" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A19" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="B19" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="C19" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="D19" s="4" t="s">
+      <c r="D19" s="18" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A20" s="11"/>
-      <c r="B20" s="11"/>
-      <c r="C20" s="11"/>
-      <c r="D20" s="11"/>
-    </row>
-    <row r="21" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A21" s="13" t="s">
+      <c r="E19" s="28" t="s">
+        <v>100</v>
+      </c>
+      <c r="F19" s="29" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A20" s="8"/>
+      <c r="B20" s="8"/>
+      <c r="C20" s="8"/>
+      <c r="D20" s="8"/>
+    </row>
+    <row r="21" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A21" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="B21" s="14" t="s">
+      <c r="B21" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="C21" s="14" t="s">
+      <c r="C21" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="D21" s="15" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A23" s="16" t="s">
+      <c r="D21" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="E21" s="26" t="s">
+        <v>19</v>
+      </c>
+      <c r="F21" s="27" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A23" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="B23" s="16"/>
-      <c r="C23" s="16"/>
-      <c r="D23" s="16"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A24" s="16"/>
-      <c r="B24" s="16"/>
-      <c r="C24" s="16"/>
-      <c r="D24" s="16"/>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B23" s="35"/>
+      <c r="C23" s="35"/>
+      <c r="D23" s="35"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A24" s="35"/>
+      <c r="B24" s="35"/>
+      <c r="C24" s="35"/>
+      <c r="D24" s="35"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>0</v>
       </c>
@@ -1030,68 +1318,98 @@
       <c r="D26" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A28" s="8" t="s">
+      <c r="E26" t="s">
+        <v>91</v>
+      </c>
+      <c r="F26" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A28" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B28" s="9" t="s">
+      <c r="B28" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="C28" s="9" t="s">
+      <c r="C28" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="D28" s="10" t="s">
+      <c r="D28" s="7" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A29" s="2" t="s">
+      <c r="E28" s="21" t="s">
+        <v>102</v>
+      </c>
+      <c r="F28" s="22" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A29" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="B29" s="3" t="s">
+      <c r="B29" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="C29" s="3" t="s">
+      <c r="C29" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="D29" s="4" t="s">
+      <c r="D29" s="18" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A30" s="11"/>
-      <c r="B30" s="12"/>
-      <c r="C30" s="12"/>
-      <c r="D30" s="12"/>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A31" s="8" t="s">
+      <c r="E29" s="28" t="s">
+        <v>104</v>
+      </c>
+      <c r="F29" s="29" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A30" s="8"/>
+      <c r="B30" s="9"/>
+      <c r="C30" s="9"/>
+      <c r="D30" s="9"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A31" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="B31" s="9" t="s">
+      <c r="B31" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="C31" s="9" t="s">
+      <c r="C31" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="D31" s="10" t="s">
+      <c r="D31" s="11" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A32" s="5" t="s">
+      <c r="E31" s="30" t="s">
+        <v>106</v>
+      </c>
+      <c r="F31" s="31" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A32" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B32" s="6" t="s">
+      <c r="B32" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="C32" s="6" t="s">
+      <c r="C32" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="D32" s="7" t="s">
+      <c r="D32" s="5" t="s">
         <v>50</v>
+      </c>
+      <c r="E32" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="F32" s="23" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -1104,92 +1422,127 @@
       <c r="C33" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="D33" s="4" t="s">
+      <c r="D33" s="3" t="s">
         <v>53</v>
       </c>
+      <c r="E33" s="20" t="s">
+        <v>109</v>
+      </c>
+      <c r="F33" s="19" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="34" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A34" s="11"/>
-      <c r="B34" s="11"/>
-      <c r="C34" s="11"/>
-      <c r="D34" s="11"/>
+      <c r="A34" s="8"/>
+      <c r="B34" s="8"/>
+      <c r="C34" s="8"/>
+      <c r="D34" s="8"/>
     </row>
     <row r="35" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A35" s="13" t="s">
+      <c r="A35" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="B35" s="14" t="s">
+      <c r="B35" s="16" t="s">
         <v>54</v>
       </c>
-      <c r="C35" s="14" t="s">
+      <c r="C35" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="D35" s="15" t="s">
+      <c r="D35" s="16" t="s">
         <v>26</v>
       </c>
+      <c r="E35" s="26" t="s">
+        <v>111</v>
+      </c>
+      <c r="F35" s="27" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="36" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A36" s="11"/>
-      <c r="B36" s="11"/>
-      <c r="C36" s="11"/>
-      <c r="D36" s="11"/>
+      <c r="A36" s="8"/>
+      <c r="B36" s="8"/>
+      <c r="C36" s="8"/>
+      <c r="D36" s="8"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A37" s="8" t="s">
+      <c r="A37" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B37" s="9" t="s">
+      <c r="B37" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="C37" s="9" t="s">
+      <c r="C37" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="D37" s="10" t="s">
+      <c r="D37" s="7" t="s">
         <v>33</v>
       </c>
+      <c r="E37" s="21" t="s">
+        <v>113</v>
+      </c>
+      <c r="F37" s="22" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A38" s="5" t="s">
+      <c r="A38" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B38" s="6" t="s">
+      <c r="B38" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="C38" s="6" t="s">
+      <c r="C38" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D38" s="7" t="s">
+      <c r="D38" s="5" t="s">
         <v>33</v>
       </c>
+      <c r="E38" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="F38" s="23" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A39" s="5" t="s">
+      <c r="A39" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B39" s="6" t="s">
+      <c r="B39" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="C39" s="6" t="s">
+      <c r="C39" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="D39" s="7" t="s">
+      <c r="D39" s="5" t="s">
         <v>33</v>
       </c>
+      <c r="E39" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="F39" s="23" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A40" s="5" t="s">
+      <c r="A40" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="B40" s="6" t="s">
+      <c r="B40" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="C40" s="6" t="s">
+      <c r="C40" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="D40" s="7" t="s">
+      <c r="D40" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="F40" s="1"/>
+      <c r="E40" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="F40" s="32" t="s">
+        <v>115</v>
+      </c>
     </row>
     <row r="41" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A41" s="2" t="s">
@@ -1201,28 +1554,40 @@
       <c r="C41" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="D41" s="4" t="s">
+      <c r="D41" s="3" t="s">
         <v>61</v>
       </c>
+      <c r="E41" s="20" t="s">
+        <v>116</v>
+      </c>
+      <c r="F41" s="19" t="s">
+        <v>117</v>
+      </c>
     </row>
     <row r="42" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A42" s="11"/>
-      <c r="B42" s="11"/>
-      <c r="C42" s="11"/>
-      <c r="D42" s="11"/>
+      <c r="A42" s="8"/>
+      <c r="B42" s="8"/>
+      <c r="C42" s="8"/>
+      <c r="D42" s="8"/>
     </row>
     <row r="43" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A43" s="13" t="s">
+      <c r="A43" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="B43" s="14" t="s">
+      <c r="B43" s="16" t="s">
         <v>62</v>
       </c>
-      <c r="C43" s="14" t="s">
+      <c r="C43" s="16" t="s">
         <v>58</v>
       </c>
-      <c r="D43" s="15" t="s">
+      <c r="D43" s="16" t="s">
         <v>33</v>
+      </c>
+      <c r="E43" s="26" t="s">
+        <v>118</v>
+      </c>
+      <c r="F43" s="27" t="s">
+        <v>119</v>
       </c>
     </row>
   </sheetData>
@@ -1240,28 +1605,30 @@
   <dimension ref="A1:G43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+      <selection activeCell="L39" sqref="L39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
     <col min="2" max="4" width="15.7265625" customWidth="1"/>
+    <col min="5" max="5" width="12.1796875" customWidth="1"/>
+    <col min="6" max="6" width="12.54296875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A2" s="16"/>
-      <c r="B2" s="16"/>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
+      <c r="A2" s="35"/>
+      <c r="B2" s="35"/>
+      <c r="C2" s="35"/>
+      <c r="D2" s="35"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
@@ -1276,20 +1643,32 @@
       <c r="D4" t="s">
         <v>4</v>
       </c>
+      <c r="E4" t="s">
+        <v>91</v>
+      </c>
+      <c r="F4" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="5" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="C6" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="D6" s="10" t="s">
+      <c r="D6" s="11" t="s">
         <v>26</v>
+      </c>
+      <c r="E6" s="30" t="s">
+        <v>120</v>
+      </c>
+      <c r="F6" s="31" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -1302,41 +1681,59 @@
       <c r="C7" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="D7" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E7" s="20" t="s">
+        <v>122</v>
+      </c>
+      <c r="F7" s="19" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="11"/>
-      <c r="B8" s="12"/>
-      <c r="C8" s="12"/>
-      <c r="D8" s="12"/>
+      <c r="A8" s="8"/>
+      <c r="B8" s="9"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A9" s="8" t="s">
+      <c r="A9" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="9" t="s">
+      <c r="B9" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="C9" s="9" t="s">
+      <c r="C9" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="D9" s="10" t="s">
+      <c r="D9" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="E9" s="30" t="s">
+        <v>123</v>
+      </c>
+      <c r="F9" s="31" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C10" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="D10" s="7" t="s">
+      <c r="D10" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="F10" s="23" t="s">
         <v>18</v>
       </c>
       <c r="G10" s="1"/>
@@ -1351,93 +1748,129 @@
       <c r="C11" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="D11" s="3" t="s">
         <v>20</v>
       </c>
+      <c r="E11" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="F11" s="19" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="12" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A12" s="11"/>
-      <c r="B12" s="11"/>
-      <c r="C12" s="11"/>
-      <c r="D12" s="11"/>
+      <c r="A12" s="8"/>
+      <c r="B12" s="8"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
     </row>
     <row r="13" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="13" t="s">
+      <c r="A13" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="B13" s="14" t="s">
+      <c r="B13" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="C13" s="14" t="s">
+      <c r="C13" s="16" t="s">
         <v>68</v>
       </c>
-      <c r="D13" s="15" t="s">
+      <c r="D13" s="33" t="s">
+        <v>18</v>
+      </c>
+      <c r="E13" s="26" t="s">
+        <v>123</v>
+      </c>
+      <c r="F13" s="27" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A14" s="11"/>
-      <c r="B14" s="11"/>
-      <c r="C14" s="11"/>
-      <c r="D14" s="11"/>
+      <c r="A14" s="8"/>
+      <c r="B14" s="8"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A15" s="8" t="s">
+      <c r="A15" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B15" s="9" t="s">
+      <c r="B15" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="C15" s="9" t="s">
+      <c r="C15" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="D15" s="10" t="s">
+      <c r="D15" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E15" s="21" t="s">
+        <v>98</v>
+      </c>
+      <c r="F15" s="22" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A16" s="5" t="s">
+      <c r="A16" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="B16" s="6" t="s">
+      <c r="B16" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="C16" s="6" t="s">
+      <c r="C16" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="D16" s="7" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A17" s="5" t="s">
+      <c r="D16" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="E16" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="F16" s="25" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A17" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B17" s="6" t="s">
+      <c r="B17" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C17" s="6" t="s">
+      <c r="C17" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="D17" s="7" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A18" s="5" t="s">
+      <c r="D17" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="F17" s="23" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A18" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B18" s="6" t="s">
+      <c r="B18" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="C18" s="6" t="s">
+      <c r="C18" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="D18" s="7" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D18" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="F18" s="23" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A19" s="2" t="s">
         <v>5</v>
       </c>
@@ -1447,45 +1880,57 @@
       <c r="C19" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="D19" s="4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A20" s="11"/>
-      <c r="B20" s="11"/>
-      <c r="C20" s="11"/>
-      <c r="D20" s="11"/>
-    </row>
-    <row r="21" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A21" s="13" t="s">
+      <c r="D19" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E19" s="20" t="s">
+        <v>125</v>
+      </c>
+      <c r="F19" s="19" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A20" s="8"/>
+      <c r="B20" s="8"/>
+      <c r="C20" s="8"/>
+      <c r="D20" s="8"/>
+    </row>
+    <row r="21" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A21" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="B21" s="14" t="s">
+      <c r="B21" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="C21" s="14" t="s">
+      <c r="C21" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="D21" s="15" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A23" s="16" t="s">
+      <c r="D21" s="33" t="s">
+        <v>18</v>
+      </c>
+      <c r="E21" s="26" t="s">
+        <v>19</v>
+      </c>
+      <c r="F21" s="27" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A23" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="B23" s="16"/>
-      <c r="C23" s="16"/>
-      <c r="D23" s="16"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A24" s="16"/>
-      <c r="B24" s="16"/>
-      <c r="C24" s="16"/>
-      <c r="D24" s="16"/>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B23" s="35"/>
+      <c r="C23" s="35"/>
+      <c r="D23" s="35"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A24" s="35"/>
+      <c r="B24" s="35"/>
+      <c r="C24" s="35"/>
+      <c r="D24" s="35"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>0</v>
       </c>
@@ -1498,199 +1943,276 @@
       <c r="D26" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A28" s="8" t="s">
+      <c r="E26" t="s">
+        <v>91</v>
+      </c>
+      <c r="F26" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A28" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B28" s="9" t="s">
+      <c r="B28" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="C28" s="9" t="s">
+      <c r="C28" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="D28" s="10" t="s">
+      <c r="D28" s="7" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A29" s="2" t="s">
+      <c r="E28" s="21" t="s">
+        <v>126</v>
+      </c>
+      <c r="F28" s="22" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A29" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="B29" s="3" t="s">
+      <c r="B29" s="18" t="s">
         <v>75</v>
       </c>
-      <c r="C29" s="3" t="s">
+      <c r="C29" s="18" t="s">
         <v>76</v>
       </c>
-      <c r="D29" s="4" t="s">
+      <c r="D29" s="18" t="s">
         <v>77</v>
       </c>
-      <c r="E29" s="1"/>
-    </row>
-    <row r="30" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A30" s="11"/>
-      <c r="B30" s="12"/>
-      <c r="C30" s="12"/>
-      <c r="D30" s="12"/>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A31" s="8" t="s">
+      <c r="E29" s="34" t="s">
+        <v>128</v>
+      </c>
+      <c r="F29" s="29" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A30" s="8"/>
+      <c r="B30" s="9"/>
+      <c r="C30" s="9"/>
+      <c r="D30" s="9"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A31" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B31" s="9" t="s">
+      <c r="B31" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="C31" s="9" t="s">
+      <c r="C31" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="D31" s="10" t="s">
+      <c r="D31" s="7" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A32" s="5" t="s">
+      <c r="E31" s="21" t="s">
+        <v>130</v>
+      </c>
+      <c r="F31" s="22" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A32" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B32" s="6" t="s">
+      <c r="B32" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="C32" s="6" t="s">
+      <c r="C32" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="D32" s="7" t="s">
+      <c r="D32" s="5" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A33" s="2" t="s">
+      <c r="E32" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="F32" s="23" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A33" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="B33" s="3" t="s">
+      <c r="B33" s="18" t="s">
         <v>81</v>
       </c>
-      <c r="C33" s="3" t="s">
+      <c r="C33" s="18" t="s">
         <v>82</v>
       </c>
-      <c r="D33" s="4" t="s">
+      <c r="D33" s="18" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A34" s="11"/>
-      <c r="B34" s="11"/>
-      <c r="C34" s="11"/>
-      <c r="D34" s="11"/>
-    </row>
-    <row r="35" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A35" s="13" t="s">
+      <c r="E33" s="28" t="s">
+        <v>133</v>
+      </c>
+      <c r="F33" s="29" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A34" s="8"/>
+      <c r="B34" s="8"/>
+      <c r="C34" s="8"/>
+      <c r="D34" s="8"/>
+    </row>
+    <row r="35" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A35" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="B35" s="14" t="s">
+      <c r="B35" s="16" t="s">
         <v>83</v>
       </c>
-      <c r="C35" s="14" t="s">
+      <c r="C35" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="D35" s="15" t="s">
+      <c r="D35" s="16" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A36" s="11"/>
-      <c r="B36" s="11"/>
-      <c r="C36" s="11"/>
-      <c r="D36" s="11"/>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A37" s="8" t="s">
+      <c r="E35" s="26" t="s">
+        <v>135</v>
+      </c>
+      <c r="F35" s="27" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A36" s="8"/>
+      <c r="B36" s="8"/>
+      <c r="C36" s="8"/>
+      <c r="D36" s="8"/>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A37" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B37" s="9" t="s">
+      <c r="B37" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="C37" s="9" t="s">
+      <c r="C37" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="D37" s="10" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A38" s="5" t="s">
+      <c r="D37" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E37" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="F37" s="22" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A38" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B38" s="6" t="s">
+      <c r="B38" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="C38" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D38" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E38" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="F38" s="23" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A39" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="C39" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D39" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E39" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="F39" s="23" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A40" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B40" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="C38" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="D38" s="7" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A39" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B39" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="C39" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D39" s="7" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A40" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B40" s="6" t="s">
+      <c r="C40" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="C40" s="6" t="s">
+      <c r="D40" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="D40" s="7" t="s">
+      <c r="E40" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="F40" s="23" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A41" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="B41" s="18" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A41" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B41" s="3" t="s">
+      <c r="C41" s="18" t="s">
         <v>89</v>
       </c>
-      <c r="C41" s="3" t="s">
+      <c r="D41" s="18" t="s">
         <v>90</v>
       </c>
-      <c r="D41" s="4" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A42" s="11"/>
-      <c r="B42" s="11"/>
-      <c r="C42" s="11"/>
-      <c r="D42" s="11"/>
-    </row>
-    <row r="43" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A43" s="13" t="s">
+      <c r="E41" s="28" t="s">
+        <v>142</v>
+      </c>
+      <c r="F41" s="29" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A42" s="8"/>
+      <c r="B42" s="8"/>
+      <c r="C42" s="8"/>
+      <c r="D42" s="8"/>
+    </row>
+    <row r="43" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A43" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="B43" s="14" t="s">
+      <c r="B43" s="16" t="s">
         <v>78</v>
       </c>
-      <c r="C43" s="14" t="s">
+      <c r="C43" s="16" t="s">
         <v>68</v>
       </c>
-      <c r="D43" s="15" t="s">
-        <v>18</v>
+      <c r="D43" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="E43" s="26" t="s">
+        <v>144</v>
+      </c>
+      <c r="F43" s="27" t="s">
+        <v>145</v>
       </c>
     </row>
   </sheetData>

</xml_diff>